<commit_message>
Updating the requirements list
</commit_message>
<xml_diff>
--- a/org.panorama-research.waters-2019.requirements/waters-challenge-2019-requirements.xlsx
+++ b/org.panorama-research.waters-2019.requirements/waters-challenge-2019-requirements.xlsx
@@ -42,22 +42,22 @@
         <r>
           <rPr>
             <b/>
-            <sz val="9"/>
+            <sz val="12"/>
             <color indexed="81"/>
             <rFont val="Segoe UI"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">Bjoern Koopmann
-</t>
+          <t>Bjoern Koopmann:</t>
         </r>
         <r>
           <rPr>
-            <sz val="9"/>
+            <sz val="12"/>
             <color indexed="81"/>
             <rFont val="Segoe UI"/>
             <family val="2"/>
           </rPr>
-          <t>TODO: Add timing requirements</t>
+          <t xml:space="preserve">
+Detection after driving for 5 m at 50 km/h</t>
         </r>
       </text>
     </comment>
@@ -66,7 +66,7 @@
         <r>
           <rPr>
             <b/>
-            <sz val="9"/>
+            <sz val="12"/>
             <color indexed="81"/>
             <rFont val="Segoe UI"/>
             <family val="2"/>
@@ -75,13 +75,14 @@
         </r>
         <r>
           <rPr>
-            <sz val="9"/>
+            <sz val="12"/>
             <color indexed="81"/>
             <rFont val="Segoe UI"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-TODO: Add timing requirements</t>
+Remains unchanged
+Do we have to define "within a dangerous zone" more precisely?</t>
         </r>
       </text>
     </comment>
@@ -90,7 +91,7 @@
         <r>
           <rPr>
             <b/>
-            <sz val="9"/>
+            <sz val="12"/>
             <color indexed="81"/>
             <rFont val="Segoe UI"/>
             <family val="2"/>
@@ -99,22 +100,22 @@
         </r>
         <r>
           <rPr>
-            <sz val="9"/>
+            <sz val="12"/>
             <color indexed="81"/>
             <rFont val="Segoe UI"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-TODO: Add timing requirements</t>
+Remains unchanged</t>
         </r>
       </text>
     </comment>
-    <comment ref="B39" authorId="0" shapeId="0">
+    <comment ref="B30" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
             <b/>
-            <sz val="9"/>
+            <sz val="12"/>
             <color indexed="81"/>
             <rFont val="Segoe UI"/>
             <family val="2"/>
@@ -123,22 +124,22 @@
         </r>
         <r>
           <rPr>
-            <sz val="9"/>
+            <sz val="12"/>
             <color indexed="81"/>
             <rFont val="Segoe UI"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-TODO: Add timing requirements</t>
+Added a default value. A delay of 50 ms should be sufficent from my opinion.</t>
         </r>
       </text>
     </comment>
-    <comment ref="B43" authorId="0" shapeId="0">
+    <comment ref="B46" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
             <b/>
-            <sz val="9"/>
+            <sz val="12"/>
             <color indexed="81"/>
             <rFont val="Segoe UI"/>
             <family val="2"/>
@@ -147,133 +148,13 @@
         </r>
         <r>
           <rPr>
-            <sz val="9"/>
+            <sz val="12"/>
             <color indexed="81"/>
             <rFont val="Segoe UI"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-TODO: Add timing requirements</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B45" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Segoe UI"/>
-            <family val="2"/>
-          </rPr>
-          <t>Bjoern Koopmann:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Segoe UI"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-TODO: Add timing requirements</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B46" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Segoe UI"/>
-            <family val="2"/>
-          </rPr>
-          <t>Bjoern Koopmann:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Segoe UI"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-TODO: Add timing requirements</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B48" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Segoe UI"/>
-            <family val="2"/>
-          </rPr>
-          <t>Bjoern Koopmann:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Segoe UI"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-TODO: Add timing requirements</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B50" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Segoe UI"/>
-            <family val="2"/>
-          </rPr>
-          <t>Bjoern Koopmann:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Segoe UI"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-TODO: Add timing requirements</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B51" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Segoe UI"/>
-            <family val="2"/>
-          </rPr>
-          <t>Bjoern Koopmann:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Segoe UI"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-TODO: Add timing requirements</t>
+Added two exemplary timing requirements that could be derived from the specification of an interacting system.</t>
         </r>
       </text>
     </comment>
@@ -282,7 +163,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="129">
   <si>
     <t>ID</t>
   </si>
@@ -482,9 +363,6 @@
     <t>1.2</t>
   </si>
   <si>
-    <t>The system shall detect vulnerable road users in time, i.e. within X ms.</t>
-  </si>
-  <si>
     <t>The system shall be able to detect vulnerable road users.</t>
   </si>
   <si>
@@ -542,16 +420,7 @@
     <t>The system shall be able to detect when the steering commands are not on time.</t>
   </si>
   <si>
-    <t>The system shall ensure that steering commands are provided within X ms.</t>
-  </si>
-  <si>
-    <t>The systen shall prevent unintended leaving of the road.</t>
-  </si>
-  <si>
     <t>The system shall have more than one sensor used to identify the road lane.</t>
-  </si>
-  <si>
-    <t>The system shall do a sanity check on the calculated speed profile to avoid leaving the road un-intentionally.</t>
   </si>
   <si>
     <t>The system shall identify and mitigate ECU failures.</t>
@@ -607,6 +476,81 @@
   </si>
   <si>
     <t>The system shall start breaking within 50 ms after the vulnerable user is detected within a dangerous zone.</t>
+  </si>
+  <si>
+    <t>A-1</t>
+  </si>
+  <si>
+    <t>A-2</t>
+  </si>
+  <si>
+    <t>The vehicle must drive at a maximum speed of 50 km/h.</t>
+  </si>
+  <si>
+    <t>A-3</t>
+  </si>
+  <si>
+    <t>The system shall stop safely after detecting vulnerable road users at a distance of at least 20 m.</t>
+  </si>
+  <si>
+    <t>The system shall reduce its speed to a maximum to reduce the impact energy after detecting vulnerable road users less than 20 m away.</t>
+  </si>
+  <si>
+    <t>The system shall detect vulnerable road users in time, i.e. within 350 ms.</t>
+  </si>
+  <si>
+    <t>The system shall ensure that steering commands are provided within 50 ms.</t>
+  </si>
+  <si>
+    <t>5.4.1</t>
+  </si>
+  <si>
+    <t>5.4.2</t>
+  </si>
+  <si>
+    <t>The system shall provide longitudinal control value updates every 15 ms.</t>
+  </si>
+  <si>
+    <t>The system shall provide lateral control value updates every 5 ms.</t>
+  </si>
+  <si>
+    <t>Functional</t>
+  </si>
+  <si>
+    <t>]0,350] ms</t>
+  </si>
+  <si>
+    <t>Safety</t>
+  </si>
+  <si>
+    <t>Safety mechanism (redundancy)</t>
+  </si>
+  <si>
+    <t>Safety mechanism (monitoring)</t>
+  </si>
+  <si>
+    <t>Safety mechanism (warning)</t>
+  </si>
+  <si>
+    <t>]0,50] ms</t>
+  </si>
+  <si>
+    <t>The system shall do a sanity check on the calculated speed profile to avoid leaving the road unintentionally.</t>
+  </si>
+  <si>
+    <t>Safety mechanism (check)</t>
+  </si>
+  <si>
+    <t>]0,100] ms</t>
+  </si>
+  <si>
+    <t>every 15 ms</t>
+  </si>
+  <si>
+    <t>every 5 ms</t>
+  </si>
+  <si>
+    <t>The system shall prevent unintended leaving of the road.</t>
   </si>
 </sst>
 </file>
@@ -622,19 +566,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="16"/>
       <color theme="1"/>
       <name val="Helvetica"/>
@@ -644,6 +575,19 @@
       <sz val="16"/>
       <color theme="0"/>
       <name val="Helvetica"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="7">
@@ -696,22 +640,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1026,211 +971,274 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AK63"/>
+  <dimension ref="A1:AK75"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="20.25" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.875" style="2"/>
-    <col min="2" max="2" width="155.5" style="2" customWidth="1"/>
+    <col min="2" max="2" width="162.375" style="2" customWidth="1"/>
     <col min="3" max="3" width="16.75" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="15.875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="42.625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="39" style="2" customWidth="1"/>
     <col min="7" max="7" width="29.625" style="2" customWidth="1"/>
     <col min="8" max="16384" width="10.875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2"/>
+      <c r="R4" s="2"/>
+      <c r="S4" s="2"/>
+      <c r="T4" s="2"/>
+      <c r="U4" s="2"/>
+      <c r="V4" s="2"/>
+      <c r="W4" s="2"/>
+      <c r="X4" s="2"/>
+      <c r="Y4" s="2"/>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D5" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D6" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="9" t="s">
+      <c r="D7" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A8" s="8" t="s">
         <v>65</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>66</v>
+        <v>110</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="E8" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>2</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D10" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>8</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>118</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>8</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>119</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>8</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>120</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>8</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>120</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>8</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>120</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>8</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="17" spans="1:37" x14ac:dyDescent="0.3">
@@ -1241,10 +1249,13 @@
         <v>3</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>8</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="19" spans="1:37" x14ac:dyDescent="0.3">
@@ -1252,13 +1263,16 @@
         <v>26</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>13</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="20" spans="1:37" x14ac:dyDescent="0.3">
@@ -1266,10 +1280,13 @@
         <v>40</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>8</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="21" spans="1:37" x14ac:dyDescent="0.3">
@@ -1277,10 +1294,13 @@
         <v>41</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>8</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>120</v>
       </c>
       <c r="G21" s="2" t="s">
         <v>20</v>
@@ -1291,10 +1311,13 @@
         <v>42</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>8</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>121</v>
       </c>
       <c r="G22" s="2" t="s">
         <v>20</v>
@@ -1305,10 +1328,13 @@
         <v>43</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>8</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="25" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -1316,18 +1342,23 @@
         <v>4</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="26" spans="1:37" s="10" customFormat="1" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="26" spans="1:37" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
         <v>27</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
+      <c r="D26" s="3" t="s">
+        <v>116</v>
+      </c>
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
@@ -1362,15 +1393,17 @@
       <c r="AJ26" s="3"/>
       <c r="AK26" s="3"/>
     </row>
-    <row r="27" spans="1:37" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:37" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
         <v>28</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
+      <c r="D27" s="3" t="s">
+        <v>116</v>
+      </c>
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
@@ -1405,12 +1438,12 @@
       <c r="AJ27" s="3"/>
       <c r="AK27" s="3"/>
     </row>
-    <row r="28" spans="1:37" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:37" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
         <v>29</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>8</v>
@@ -1418,7 +1451,9 @@
       <c r="D28" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E28" s="3"/>
+      <c r="E28" s="3" t="s">
+        <v>125</v>
+      </c>
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>
@@ -1452,18 +1487,18 @@
       <c r="AJ28" s="3"/>
       <c r="AK28" s="3"/>
     </row>
-    <row r="29" spans="1:37" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:37" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B29" s="4" t="s">
-        <v>85</v>
+      <c r="B29" s="3" t="s">
+        <v>84</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>13</v>
+        <v>120</v>
       </c>
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
@@ -1501,12 +1536,12 @@
       <c r="AJ29" s="3"/>
       <c r="AK29" s="3"/>
     </row>
-    <row r="30" spans="1:37" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:37" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
         <v>46</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>86</v>
+        <v>111</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>8</v>
@@ -1514,7 +1549,9 @@
       <c r="D30" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E30" s="3"/>
+      <c r="E30" s="3" t="s">
+        <v>122</v>
+      </c>
       <c r="F30" s="3"/>
       <c r="G30" s="3"/>
       <c r="H30" s="3"/>
@@ -1548,17 +1585,19 @@
       <c r="AJ30" s="3"/>
       <c r="AK30" s="3"/>
     </row>
-    <row r="31" spans="1:37" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:37" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
         <v>44</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>87</v>
+        <v>128</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D31" s="3"/>
+      <c r="D31" s="3" t="s">
+        <v>116</v>
+      </c>
       <c r="E31" s="3"/>
       <c r="F31" s="3"/>
       <c r="G31" s="3"/>
@@ -1593,17 +1632,19 @@
       <c r="AJ31" s="3"/>
       <c r="AK31" s="3"/>
     </row>
-    <row r="32" spans="1:37" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:37" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
         <v>57</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D32" s="3"/>
+      <c r="D32" s="3" t="s">
+        <v>119</v>
+      </c>
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
       <c r="G32" s="3"/>
@@ -1638,17 +1679,19 @@
       <c r="AJ32" s="3"/>
       <c r="AK32" s="3"/>
     </row>
-    <row r="33" spans="1:37" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:37" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
         <v>58</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D33" s="3"/>
+      <c r="D33" s="3" t="s">
+        <v>120</v>
+      </c>
       <c r="E33" s="3"/>
       <c r="F33" s="3"/>
       <c r="G33" s="3" t="s">
@@ -1685,17 +1728,19 @@
       <c r="AJ33" s="3"/>
       <c r="AK33" s="3"/>
     </row>
-    <row r="34" spans="1:37" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:37" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
         <v>59</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D34" s="3"/>
+      <c r="D34" s="3" t="s">
+        <v>121</v>
+      </c>
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
       <c r="G34" s="3" t="s">
@@ -1732,17 +1777,19 @@
       <c r="AJ34" s="3"/>
       <c r="AK34" s="3"/>
     </row>
-    <row r="35" spans="1:37" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:37" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
         <v>60</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>89</v>
+        <v>123</v>
       </c>
       <c r="C35" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D35" s="3"/>
+      <c r="D35" s="3" t="s">
+        <v>124</v>
+      </c>
       <c r="E35" s="3"/>
       <c r="F35" s="3"/>
       <c r="G35" s="3"/>
@@ -1777,17 +1824,19 @@
       <c r="AJ35" s="3"/>
       <c r="AK35" s="3"/>
     </row>
-    <row r="36" spans="1:37" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:37" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
         <v>61</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D36" s="3"/>
+      <c r="D36" s="3" t="s">
+        <v>120</v>
+      </c>
       <c r="E36" s="3"/>
       <c r="F36" s="3"/>
       <c r="G36" s="3"/>
@@ -1822,17 +1871,19 @@
       <c r="AJ36" s="3"/>
       <c r="AK36" s="3"/>
     </row>
-    <row r="37" spans="1:37" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:37" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
         <v>62</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C37" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D37" s="3"/>
+      <c r="D37" s="3" t="s">
+        <v>120</v>
+      </c>
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
       <c r="G37" s="2" t="s">
@@ -1869,17 +1920,19 @@
       <c r="AJ37" s="3"/>
       <c r="AK37" s="3"/>
     </row>
-    <row r="38" spans="1:37" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:37" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
         <v>63</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C38" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D38" s="3"/>
+      <c r="D38" s="3" t="s">
+        <v>121</v>
+      </c>
       <c r="E38" s="3"/>
       <c r="F38" s="3"/>
       <c r="G38" s="2" t="s">
@@ -1916,18 +1969,18 @@
       <c r="AJ38" s="3"/>
       <c r="AK38" s="3"/>
     </row>
-    <row r="39" spans="1:37" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:37" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="B39" s="4" t="s">
-        <v>85</v>
+      <c r="B39" s="3" t="s">
+        <v>84</v>
       </c>
       <c r="C39" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>13</v>
+        <v>120</v>
       </c>
       <c r="E39" s="3"/>
       <c r="F39" s="3"/>
@@ -1970,7 +2023,10 @@
         <v>5</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>91</v>
+        <v>87</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="42" spans="1:37" x14ac:dyDescent="0.3">
@@ -1978,15 +2034,21 @@
         <v>30</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>92</v>
+        <v>88</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="43" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B43" s="4" t="s">
-        <v>93</v>
+      <c r="B43" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="44" spans="1:37" x14ac:dyDescent="0.3">
@@ -1994,209 +2056,318 @@
         <v>32</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>94</v>
+        <v>90</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="45" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B45" s="4" t="s">
-        <v>95</v>
+      <c r="B45" s="3" t="s">
+        <v>91</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="46" spans="1:37" ht="60.75" x14ac:dyDescent="0.3">
-      <c r="A46" s="2" t="s">
+      <c r="D45" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="46" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A46" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="47" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A47" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="48" spans="1:37" ht="60.75" x14ac:dyDescent="0.3">
+      <c r="A48" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B46" s="5" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="47" spans="1:37" x14ac:dyDescent="0.3">
-      <c r="A47" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B47" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="48" spans="1:37" x14ac:dyDescent="0.3">
-      <c r="A48" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B48" s="4" t="s">
-        <v>98</v>
+      <c r="B48" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>99</v>
+        <v>93</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B50" s="4" t="s">
-        <v>100</v>
+        <v>36</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B51" s="4" t="s">
-        <v>101</v>
+        <v>37</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>102</v>
+        <v>96</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G53" s="2" t="s">
-        <v>17</v>
+        <v>97</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
-        <v>50</v>
+        <v>31</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G54" s="2" t="s">
-        <v>17</v>
+        <v>98</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>106</v>
+        <v>72</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="D55" s="2" t="s">
+        <v>120</v>
+      </c>
       <c r="G55" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>105</v>
+        <v>73</v>
       </c>
       <c r="C56" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="D56" s="2" t="s">
+        <v>119</v>
+      </c>
       <c r="G56" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>75</v>
+        <v>102</v>
       </c>
       <c r="C57" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="D57" s="2" t="s">
+        <v>120</v>
+      </c>
       <c r="G57" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>76</v>
+        <v>101</v>
       </c>
       <c r="C58" s="2" t="s">
         <v>8</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="G58" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>90</v>
+        <v>74</v>
       </c>
       <c r="C59" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="D59" s="2" t="s">
+        <v>120</v>
+      </c>
       <c r="G59" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C60" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G60" s="2" t="s">
-        <v>20</v>
+      <c r="D60" s="2" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="C61" s="2" t="s">
         <v>8</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="G61" s="2" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="G62" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A63" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A64" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B62" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="C62" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B63" s="3"/>
+      <c r="B64" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B65" s="3"/>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A73" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A74" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A75" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>108</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>